<commit_message>
Load Data To DashBoard
</commit_message>
<xml_diff>
--- a/Data/Task Manager.xlsx
+++ b/Data/Task Manager.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Task Manager\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA02778-AA0E-4FBF-988E-9E6071D29828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECD558D-2514-4EE3-8A93-33BA44434C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="619" xr2:uid="{5379E9EA-E08B-4790-8D6B-9DBF20DA1D4B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
+    <sheet name="Task Manager" sheetId="1" r:id="rId1"/>
+    <sheet name="Phân Chia Công Việc" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>USER</t>
   </si>
@@ -156,6 +157,57 @@
   </si>
   <si>
     <t>IDAssignment</t>
+  </si>
+  <si>
+    <t>MSSV</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Phong</t>
+  </si>
+  <si>
+    <t>Lầu Hoàng Nguyên</t>
+  </si>
+  <si>
+    <t>Nguyễn Thành Nhân</t>
+  </si>
+  <si>
+    <t>Võ Đình Thiên Phú</t>
+  </si>
+  <si>
+    <t>Sửa Database</t>
+  </si>
+  <si>
+    <t>Đăng Nhập, Đăng Ký, Xác thực và ủy quyền người dùng bằng OAuth 2.0 đăng nhập bằng Google</t>
+  </si>
+  <si>
+    <t>Báo Cáo</t>
+  </si>
+  <si>
+    <t>Phạm Văn Phước</t>
+  </si>
+  <si>
+    <t>Chức Năng Chuyển Đổi Status</t>
+  </si>
+  <si>
+    <t>Task Progress</t>
+  </si>
+  <si>
+    <t>HỌ &amp; TÊN</t>
+  </si>
+  <si>
+    <t>CÔNG VIỆC</t>
+  </si>
+  <si>
+    <t>ĐÁNH GIÁ</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>ADD, MOVE</t>
   </si>
 </sst>
 </file>
@@ -222,7 +274,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,6 +311,24 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -598,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67DF446-5E0B-4A76-9DA7-A336C74DB690}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -821,11 +891,47 @@
     <row r="10" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1">
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" ht="30" customHeight="1"/>
-    <row r="13" spans="1:12" ht="30" customHeight="1"/>
+    <row r="11" spans="1:12" ht="30" customHeight="1"/>
+    <row r="12" spans="1:12" ht="30" customHeight="1">
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1">
+      <c r="B13" s="13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="14" spans="1:12" ht="30" customHeight="1"/>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="F15" s="3"/>
@@ -843,4 +949,131 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5BE7BF-E443-48E8-83ED-DBE55F694A85}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="24.26953125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="59.54296875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" style="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" customHeight="1">
+      <c r="A2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="17">
+        <v>2180607802</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4" ht="45" customHeight="1">
+      <c r="A3" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="17">
+        <v>2180607824</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="18">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" customHeight="1">
+      <c r="A4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="17">
+        <v>2180607874</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:4" ht="45" customHeight="1">
+      <c r="A5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="17">
+        <v>2180607177</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="45" customHeight="1">
+      <c r="A6" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="17">
+        <v>2180609103</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:4" ht="30" customHeight="1"/>
+    <row r="12" spans="1:4" ht="30" customHeight="1"/>
+    <row r="13" spans="1:4" ht="30" customHeight="1"/>
+    <row r="14" spans="1:4" ht="30" customHeight="1"/>
+    <row r="15" spans="1:4" ht="30" customHeight="1"/>
+    <row r="16" spans="1:4" ht="30" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>